<commit_message>
RTTBC24 Week 5 Noms (DEL)
</commit_message>
<xml_diff>
--- a/calendar-import-files/Gallop-Draft-Tasks-for-Google-Calendar.xlsx
+++ b/calendar-import-files/Gallop-Draft-Tasks-for-Google-Calendar.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/299f8723705ec823/Webmaster/gallop-racing.com/calendar-import-files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="46" documentId="8_{17A1D9B9-8994-4361-99E0-CCA1520F2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2BA32203-BE8F-4FB1-B789-448BB610C646}"/>
+  <xr:revisionPtr revIDLastSave="47" documentId="8_{17A1D9B9-8994-4361-99E0-CCA1520F2178}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5821CA79-25DA-4136-B824-19E2171D9247}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{27DBC710-212C-4B60-B927-B9EE36866F81}"/>
   </bookViews>
@@ -65,9 +65,6 @@
     <t>All Stables Closed for Viewing</t>
   </si>
   <si>
-    <t>Power Horse Selection Available</t>
-  </si>
-  <si>
     <t>RTTBC24 Draft #2 Opens</t>
   </si>
   <si>
@@ -75,6 +72,9 @@
   </si>
   <si>
     <t>RTTBC24 Draft #2 Closes</t>
+  </si>
+  <si>
+    <t>Power Pick Selection Available</t>
   </si>
 </sst>
 </file>
@@ -462,7 +462,7 @@
   <dimension ref="A1:H169"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -505,7 +505,7 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B2" s="1">
         <v>45468</v>
@@ -525,7 +525,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B3" s="1">
         <v>45468</v>
@@ -553,7 +553,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="B5" s="1">
         <v>45468</v>
@@ -567,7 +567,7 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B6" s="1">
         <v>45472</v>

</xml_diff>